<commit_message>
Attempting a combined version for fetching emails and cleaning them.
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/Logistic Regression Tests/Logistic Regression Model Results.xlsx
+++ b/Jeremy Thesis/Logistic Regression Tests/Logistic Regression Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255C53F4-C114-46F4-9FAE-E8B34BCF15A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F83B2E-371B-46DD-B84B-07FC6E5E44CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F96A09BA-D82A-4ECF-98D0-BA16504C11B9}"/>
   </bookViews>
@@ -552,12 +552,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mj-ea"/>
@@ -584,12 +581,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mj-ea"/>
@@ -941,12 +935,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -973,12 +964,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1011,12 +999,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1075,12 +1060,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1107,12 +1089,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1139,12 +1118,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1181,12 +1157,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -1221,7 +1194,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1500">
+        <a:defRPr sz="1500" b="1">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
           <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
           <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
         </a:defRPr>

</xml_diff>